<commit_message>
(m)cpu24--add cond flow && add data-conflict detection
</commit_message>
<xml_diff>
--- a/cpu.circ/2020-3-12.xlsx
+++ b/cpu.circ/2020-3-12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\大三下\组成原理春季课程设计\cpu+版本管理\cpu.circ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1434E7-A7D2-4C7C-A731-CB2FB171BA33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EDCF27-326E-4CF8-955D-2042CCC4A5CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13860" yWindow="2772" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="真值表" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">控制信号表达式生成!$A$1:$AJ$36</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">真值表!$A$1:$AL$25</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="124">
   <si>
     <t>#</t>
   </si>
@@ -857,6 +857,14 @@
     <t>X</t>
     <phoneticPr fontId="28" type="noConversion"/>
   </si>
+  <si>
+    <t>R1_USED</t>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2_USED</t>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1097,7 +1105,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1158,8 +1166,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1341,11 +1361,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1546,11 +1594,43 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2073,27 +2153,27 @@
   </sheetPr>
   <dimension ref="A1:AR61"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AJ24" sqref="AJ24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AN23" sqref="AN23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" style="32" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="32" customWidth="1"/>
-    <col min="5" max="9" width="4.6640625" style="32" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="4.21875" style="32" hidden="1" customWidth="1"/>
-    <col min="11" max="16" width="4.6640625" style="32" hidden="1" customWidth="1"/>
-    <col min="17" max="19" width="3.6640625" style="32" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="3.77734375" style="32" hidden="1" customWidth="1"/>
-    <col min="21" max="31" width="6.6640625" style="65" customWidth="1"/>
-    <col min="32" max="33" width="6.6640625" style="66" customWidth="1"/>
-    <col min="34" max="44" width="6.6640625" style="67" customWidth="1"/>
+    <col min="1" max="1" width="3.875" customWidth="1"/>
+    <col min="2" max="2" width="8.625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="11.25" style="32" customWidth="1"/>
+    <col min="4" max="4" width="10.625" style="32" customWidth="1"/>
+    <col min="5" max="9" width="4.625" style="32" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="4.25" style="32" hidden="1" customWidth="1"/>
+    <col min="11" max="16" width="4.625" style="32" hidden="1" customWidth="1"/>
+    <col min="17" max="19" width="3.625" style="32" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="3.75" style="32" hidden="1" customWidth="1"/>
+    <col min="21" max="31" width="6.625" style="65" customWidth="1"/>
+    <col min="32" max="33" width="6.625" style="66" customWidth="1"/>
+    <col min="34" max="44" width="6.625" style="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="17" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" s="17" customFormat="1" ht="24.75" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -2200,10 +2280,10 @@
         <v>119</v>
       </c>
       <c r="AJ1" s="58" t="s">
-        <v>33</v>
+        <v>122</v>
       </c>
       <c r="AK1" s="58" t="s">
-        <v>33</v>
+        <v>123</v>
       </c>
       <c r="AL1" s="58" t="s">
         <v>33</v>
@@ -2227,7 +2307,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2" s="38">
         <v>1</v>
       </c>
@@ -2325,8 +2405,12 @@
       <c r="AG2" s="60"/>
       <c r="AH2" s="61"/>
       <c r="AI2" s="61"/>
-      <c r="AJ2" s="61"/>
-      <c r="AK2" s="61"/>
+      <c r="AJ2" s="70">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="70">
+        <v>1</v>
+      </c>
       <c r="AL2" s="61"/>
       <c r="AM2" s="61"/>
       <c r="AN2" s="61"/>
@@ -2335,7 +2419,7 @@
       <c r="AQ2" s="61"/>
       <c r="AR2" s="61"/>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3" s="27">
         <v>2</v>
       </c>
@@ -2433,8 +2517,12 @@
       <c r="AG3" s="63"/>
       <c r="AH3" s="64"/>
       <c r="AI3" s="64"/>
-      <c r="AJ3" s="64"/>
-      <c r="AK3" s="64"/>
+      <c r="AJ3" s="71">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="71">
+        <v>1</v>
+      </c>
       <c r="AL3" s="64"/>
       <c r="AM3" s="64"/>
       <c r="AN3" s="64"/>
@@ -2443,7 +2531,7 @@
       <c r="AQ3" s="64"/>
       <c r="AR3" s="64"/>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" s="38">
         <v>3</v>
       </c>
@@ -2541,8 +2629,12 @@
       <c r="AG4" s="60"/>
       <c r="AH4" s="61"/>
       <c r="AI4" s="61"/>
-      <c r="AJ4" s="61"/>
-      <c r="AK4" s="61"/>
+      <c r="AJ4" s="70">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="70">
+        <v>1</v>
+      </c>
       <c r="AL4" s="61"/>
       <c r="AM4" s="61"/>
       <c r="AN4" s="61"/>
@@ -2551,7 +2643,7 @@
       <c r="AQ4" s="61"/>
       <c r="AR4" s="61"/>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" s="27">
         <v>4</v>
       </c>
@@ -2649,8 +2741,12 @@
       <c r="AG5" s="63"/>
       <c r="AH5" s="64"/>
       <c r="AI5" s="64"/>
-      <c r="AJ5" s="64"/>
-      <c r="AK5" s="64"/>
+      <c r="AJ5" s="71">
+        <v>1</v>
+      </c>
+      <c r="AK5" s="71">
+        <v>1</v>
+      </c>
       <c r="AL5" s="64"/>
       <c r="AM5" s="64"/>
       <c r="AN5" s="64"/>
@@ -2659,7 +2755,7 @@
       <c r="AQ5" s="64"/>
       <c r="AR5" s="64"/>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" s="38">
         <v>5</v>
       </c>
@@ -2757,8 +2853,12 @@
       <c r="AG6" s="60"/>
       <c r="AH6" s="61"/>
       <c r="AI6" s="61"/>
-      <c r="AJ6" s="61"/>
-      <c r="AK6" s="61"/>
+      <c r="AJ6" s="70">
+        <v>1</v>
+      </c>
+      <c r="AK6" s="70">
+        <v>1</v>
+      </c>
       <c r="AL6" s="61"/>
       <c r="AM6" s="61"/>
       <c r="AN6" s="61"/>
@@ -2767,7 +2867,7 @@
       <c r="AQ6" s="61"/>
       <c r="AR6" s="61"/>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7" s="27">
         <v>6</v>
       </c>
@@ -2865,8 +2965,12 @@
       <c r="AG7" s="63"/>
       <c r="AH7" s="64"/>
       <c r="AI7" s="64"/>
-      <c r="AJ7" s="64"/>
-      <c r="AK7" s="64"/>
+      <c r="AJ7" s="71">
+        <v>1</v>
+      </c>
+      <c r="AK7" s="71">
+        <v>1</v>
+      </c>
       <c r="AL7" s="64"/>
       <c r="AM7" s="64"/>
       <c r="AN7" s="64"/>
@@ -2875,7 +2979,7 @@
       <c r="AQ7" s="64"/>
       <c r="AR7" s="64"/>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8" s="38">
         <v>7</v>
       </c>
@@ -2973,8 +3077,12 @@
       <c r="AG8" s="60"/>
       <c r="AH8" s="61"/>
       <c r="AI8" s="61"/>
-      <c r="AJ8" s="61"/>
-      <c r="AK8" s="61"/>
+      <c r="AJ8" s="70">
+        <v>1</v>
+      </c>
+      <c r="AK8" s="70">
+        <v>1</v>
+      </c>
       <c r="AL8" s="61"/>
       <c r="AM8" s="61"/>
       <c r="AN8" s="61"/>
@@ -2983,7 +3091,7 @@
       <c r="AQ8" s="61"/>
       <c r="AR8" s="61"/>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A9" s="27">
         <v>8</v>
       </c>
@@ -3081,8 +3189,12 @@
       <c r="AG9" s="63"/>
       <c r="AH9" s="64"/>
       <c r="AI9" s="64"/>
-      <c r="AJ9" s="64"/>
-      <c r="AK9" s="64"/>
+      <c r="AJ9" s="71">
+        <v>1</v>
+      </c>
+      <c r="AK9" s="71">
+        <v>1</v>
+      </c>
       <c r="AL9" s="64"/>
       <c r="AM9" s="64"/>
       <c r="AN9" s="64"/>
@@ -3091,7 +3203,7 @@
       <c r="AQ9" s="64"/>
       <c r="AR9" s="64"/>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A10" s="38">
         <v>9</v>
       </c>
@@ -3189,8 +3301,12 @@
       <c r="AG10" s="60"/>
       <c r="AH10" s="61"/>
       <c r="AI10" s="61"/>
-      <c r="AJ10" s="61"/>
-      <c r="AK10" s="61"/>
+      <c r="AJ10" s="70">
+        <v>1</v>
+      </c>
+      <c r="AK10" s="70">
+        <v>1</v>
+      </c>
       <c r="AL10" s="61"/>
       <c r="AM10" s="61"/>
       <c r="AN10" s="61"/>
@@ -3199,7 +3315,7 @@
       <c r="AQ10" s="61"/>
       <c r="AR10" s="61"/>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A11" s="27">
         <v>10</v>
       </c>
@@ -3297,8 +3413,12 @@
       <c r="AG11" s="63"/>
       <c r="AH11" s="64"/>
       <c r="AI11" s="64"/>
-      <c r="AJ11" s="64"/>
-      <c r="AK11" s="64"/>
+      <c r="AJ11" s="71">
+        <v>1</v>
+      </c>
+      <c r="AK11" s="71">
+        <v>1</v>
+      </c>
       <c r="AL11" s="64"/>
       <c r="AM11" s="64"/>
       <c r="AN11" s="64"/>
@@ -3307,7 +3427,7 @@
       <c r="AQ11" s="64"/>
       <c r="AR11" s="64"/>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A12" s="38">
         <v>11</v>
       </c>
@@ -3405,8 +3525,12 @@
       <c r="AG12" s="60"/>
       <c r="AH12" s="61"/>
       <c r="AI12" s="61"/>
-      <c r="AJ12" s="61"/>
-      <c r="AK12" s="61"/>
+      <c r="AJ12" s="70">
+        <v>1</v>
+      </c>
+      <c r="AK12" s="70">
+        <v>1</v>
+      </c>
       <c r="AL12" s="61"/>
       <c r="AM12" s="61"/>
       <c r="AN12" s="61"/>
@@ -3415,7 +3539,7 @@
       <c r="AQ12" s="61"/>
       <c r="AR12" s="61"/>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A13" s="27">
         <v>12</v>
       </c>
@@ -3513,8 +3637,10 @@
       <c r="AG13" s="63"/>
       <c r="AH13" s="64"/>
       <c r="AI13" s="64"/>
-      <c r="AJ13" s="64"/>
-      <c r="AK13" s="64"/>
+      <c r="AJ13" s="71">
+        <v>1</v>
+      </c>
+      <c r="AK13" s="71"/>
       <c r="AL13" s="64"/>
       <c r="AM13" s="64"/>
       <c r="AN13" s="64"/>
@@ -3523,7 +3649,7 @@
       <c r="AQ13" s="64"/>
       <c r="AR13" s="64"/>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A14" s="38">
         <v>13</v>
       </c>
@@ -3619,8 +3745,12 @@
       <c r="AG14" s="60"/>
       <c r="AH14" s="61"/>
       <c r="AI14" s="61"/>
-      <c r="AJ14" s="61"/>
-      <c r="AK14" s="61"/>
+      <c r="AJ14" s="70">
+        <v>1</v>
+      </c>
+      <c r="AK14" s="70">
+        <v>1</v>
+      </c>
       <c r="AL14" s="61"/>
       <c r="AM14" s="61"/>
       <c r="AN14" s="61"/>
@@ -3629,7 +3759,7 @@
       <c r="AQ14" s="61"/>
       <c r="AR14" s="61"/>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A15" s="27">
         <v>14</v>
       </c>
@@ -3725,8 +3855,8 @@
       <c r="AG15" s="63"/>
       <c r="AH15" s="64"/>
       <c r="AI15" s="64"/>
-      <c r="AJ15" s="64"/>
-      <c r="AK15" s="64"/>
+      <c r="AJ15" s="71"/>
+      <c r="AK15" s="71"/>
       <c r="AL15" s="64"/>
       <c r="AM15" s="64"/>
       <c r="AN15" s="64"/>
@@ -3735,7 +3865,7 @@
       <c r="AQ15" s="64"/>
       <c r="AR15" s="64"/>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A16" s="38">
         <v>15</v>
       </c>
@@ -3835,8 +3965,8 @@
       </c>
       <c r="AH16" s="61"/>
       <c r="AI16" s="61"/>
-      <c r="AJ16" s="61"/>
-      <c r="AK16" s="61"/>
+      <c r="AJ16" s="70"/>
+      <c r="AK16" s="70"/>
       <c r="AL16" s="61"/>
       <c r="AM16" s="61"/>
       <c r="AN16" s="61"/>
@@ -3845,7 +3975,7 @@
       <c r="AQ16" s="61"/>
       <c r="AR16" s="61"/>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A17" s="27">
         <v>16</v>
       </c>
@@ -3943,8 +4073,12 @@
       <c r="AG17" s="63"/>
       <c r="AH17" s="64"/>
       <c r="AI17" s="64"/>
-      <c r="AJ17" s="64"/>
-      <c r="AK17" s="64"/>
+      <c r="AJ17" s="71">
+        <v>1</v>
+      </c>
+      <c r="AK17" s="71">
+        <v>1</v>
+      </c>
       <c r="AL17" s="64"/>
       <c r="AM17" s="64"/>
       <c r="AN17" s="64"/>
@@ -3953,7 +4087,7 @@
       <c r="AQ17" s="64"/>
       <c r="AR17" s="64"/>
     </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A18" s="38">
         <v>17</v>
       </c>
@@ -4051,8 +4185,12 @@
       <c r="AG18" s="60"/>
       <c r="AH18" s="61"/>
       <c r="AI18" s="61"/>
-      <c r="AJ18" s="61"/>
-      <c r="AK18" s="61"/>
+      <c r="AJ18" s="70">
+        <v>1</v>
+      </c>
+      <c r="AK18" s="70">
+        <v>1</v>
+      </c>
       <c r="AL18" s="61"/>
       <c r="AM18" s="61"/>
       <c r="AN18" s="61"/>
@@ -4061,7 +4199,7 @@
       <c r="AQ18" s="61"/>
       <c r="AR18" s="61"/>
     </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A19" s="27">
         <v>18</v>
       </c>
@@ -4161,8 +4299,10 @@
       <c r="AG19" s="63"/>
       <c r="AH19" s="64"/>
       <c r="AI19" s="64"/>
-      <c r="AJ19" s="64"/>
-      <c r="AK19" s="64"/>
+      <c r="AJ19" s="71">
+        <v>1</v>
+      </c>
+      <c r="AK19" s="71"/>
       <c r="AL19" s="64"/>
       <c r="AM19" s="64"/>
       <c r="AN19" s="64"/>
@@ -4171,7 +4311,7 @@
       <c r="AQ19" s="64"/>
       <c r="AR19" s="64"/>
     </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A20" s="38">
         <v>19</v>
       </c>
@@ -4269,8 +4409,10 @@
       <c r="AG20" s="60"/>
       <c r="AH20" s="61"/>
       <c r="AI20" s="61"/>
-      <c r="AJ20" s="61"/>
-      <c r="AK20" s="61"/>
+      <c r="AJ20" s="70">
+        <v>1</v>
+      </c>
+      <c r="AK20" s="70"/>
       <c r="AL20" s="61"/>
       <c r="AM20" s="61"/>
       <c r="AN20" s="61"/>
@@ -4279,7 +4421,7 @@
       <c r="AQ20" s="61"/>
       <c r="AR20" s="61"/>
     </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A21" s="27">
         <v>20</v>
       </c>
@@ -4379,8 +4521,10 @@
       <c r="AG21" s="63"/>
       <c r="AH21" s="64"/>
       <c r="AI21" s="64"/>
-      <c r="AJ21" s="64"/>
-      <c r="AK21" s="64"/>
+      <c r="AJ21" s="71">
+        <v>1</v>
+      </c>
+      <c r="AK21" s="71"/>
       <c r="AL21" s="64"/>
       <c r="AM21" s="64"/>
       <c r="AN21" s="64"/>
@@ -4389,7 +4533,7 @@
       <c r="AQ21" s="64"/>
       <c r="AR21" s="64"/>
     </row>
-    <row r="22" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A22" s="38">
         <v>21</v>
       </c>
@@ -4489,8 +4633,10 @@
       <c r="AG22" s="60"/>
       <c r="AH22" s="61"/>
       <c r="AI22" s="61"/>
-      <c r="AJ22" s="61"/>
-      <c r="AK22" s="61"/>
+      <c r="AJ22" s="70">
+        <v>1</v>
+      </c>
+      <c r="AK22" s="70"/>
       <c r="AL22" s="61"/>
       <c r="AM22" s="61"/>
       <c r="AN22" s="61"/>
@@ -4499,7 +4645,7 @@
       <c r="AQ22" s="61"/>
       <c r="AR22" s="61"/>
     </row>
-    <row r="23" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A23" s="27">
         <v>22</v>
       </c>
@@ -4597,8 +4743,10 @@
       <c r="AG23" s="63"/>
       <c r="AH23" s="64"/>
       <c r="AI23" s="64"/>
-      <c r="AJ23" s="64"/>
-      <c r="AK23" s="64"/>
+      <c r="AJ23" s="71">
+        <v>1</v>
+      </c>
+      <c r="AK23" s="71"/>
       <c r="AL23" s="64"/>
       <c r="AM23" s="64"/>
       <c r="AN23" s="64"/>
@@ -4607,7 +4755,7 @@
       <c r="AQ23" s="64"/>
       <c r="AR23" s="64"/>
     </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A24" s="38">
         <v>23</v>
       </c>
@@ -4709,8 +4857,12 @@
       <c r="AG24" s="60"/>
       <c r="AH24" s="61"/>
       <c r="AI24" s="61"/>
-      <c r="AJ24" s="61"/>
-      <c r="AK24" s="61"/>
+      <c r="AJ24" s="70">
+        <v>1</v>
+      </c>
+      <c r="AK24" s="70">
+        <v>1</v>
+      </c>
       <c r="AL24" s="61"/>
       <c r="AM24" s="61"/>
       <c r="AN24" s="61"/>
@@ -4719,7 +4871,7 @@
       <c r="AQ24" s="61"/>
       <c r="AR24" s="61"/>
     </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A25" s="27">
         <v>24</v>
       </c>
@@ -4819,8 +4971,12 @@
       <c r="AG25" s="63"/>
       <c r="AH25" s="64"/>
       <c r="AI25" s="64"/>
-      <c r="AJ25" s="64"/>
-      <c r="AK25" s="64"/>
+      <c r="AJ25" s="71">
+        <v>1</v>
+      </c>
+      <c r="AK25" s="71">
+        <v>1</v>
+      </c>
       <c r="AL25" s="64"/>
       <c r="AM25" s="64"/>
       <c r="AN25" s="64"/>
@@ -4829,7 +4985,7 @@
       <c r="AQ25" s="64"/>
       <c r="AR25" s="64"/>
     </row>
-    <row r="26" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A26" s="38">
         <v>25</v>
       </c>
@@ -4927,8 +5083,12 @@
       <c r="AG26" s="60"/>
       <c r="AH26" s="61"/>
       <c r="AI26" s="61"/>
-      <c r="AJ26" s="61"/>
-      <c r="AK26" s="61"/>
+      <c r="AJ26" s="61">
+        <v>1</v>
+      </c>
+      <c r="AK26" s="61">
+        <v>1</v>
+      </c>
       <c r="AL26" s="61"/>
       <c r="AM26" s="61"/>
       <c r="AN26" s="61"/>
@@ -4937,7 +5097,7 @@
       <c r="AQ26" s="61"/>
       <c r="AR26" s="61"/>
     </row>
-    <row r="27" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A27" s="27">
         <v>26</v>
       </c>
@@ -5035,7 +5195,9 @@
       <c r="AG27" s="63"/>
       <c r="AH27" s="64"/>
       <c r="AI27" s="64"/>
-      <c r="AJ27" s="64"/>
+      <c r="AJ27" s="64">
+        <v>1</v>
+      </c>
       <c r="AK27" s="64"/>
       <c r="AL27" s="64"/>
       <c r="AM27" s="64"/>
@@ -5045,7 +5207,7 @@
       <c r="AQ27" s="64"/>
       <c r="AR27" s="64"/>
     </row>
-    <row r="28" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A28" s="38">
         <v>27</v>
       </c>
@@ -5149,8 +5311,12 @@
       <c r="AI28" s="61">
         <v>1</v>
       </c>
-      <c r="AJ28" s="61"/>
-      <c r="AK28" s="61"/>
+      <c r="AJ28" s="61">
+        <v>1</v>
+      </c>
+      <c r="AK28" s="61">
+        <v>1</v>
+      </c>
       <c r="AL28" s="61"/>
       <c r="AM28" s="61"/>
       <c r="AN28" s="61"/>
@@ -5159,7 +5325,7 @@
       <c r="AQ28" s="61"/>
       <c r="AR28" s="61"/>
     </row>
-    <row r="29" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A29" s="27">
         <v>28</v>
       </c>
@@ -5257,7 +5423,9 @@
         <v>1</v>
       </c>
       <c r="AI29" s="64"/>
-      <c r="AJ29" s="64"/>
+      <c r="AJ29" s="64">
+        <v>1</v>
+      </c>
       <c r="AK29" s="64"/>
       <c r="AL29" s="64"/>
       <c r="AM29" s="64"/>
@@ -5267,7 +5435,7 @@
       <c r="AQ29" s="64"/>
       <c r="AR29" s="64"/>
     </row>
-    <row r="30" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A30" s="38">
         <v>29</v>
       </c>
@@ -5363,7 +5531,7 @@
       <c r="AQ30" s="61"/>
       <c r="AR30" s="61"/>
     </row>
-    <row r="31" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A31" s="27">
         <v>30</v>
       </c>
@@ -5459,7 +5627,7 @@
       <c r="AQ31" s="64"/>
       <c r="AR31" s="64"/>
     </row>
-    <row r="32" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A32" s="38">
         <v>31</v>
       </c>
@@ -5555,7 +5723,7 @@
       <c r="AQ32" s="61"/>
       <c r="AR32" s="61"/>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A33" s="27"/>
       <c r="B33" s="52"/>
       <c r="C33" s="46"/>
@@ -5649,7 +5817,7 @@
       <c r="AQ33" s="64"/>
       <c r="AR33" s="64"/>
     </row>
-    <row r="34" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A34" s="38"/>
       <c r="B34" s="35"/>
       <c r="C34" s="39"/>
@@ -5743,7 +5911,7 @@
       <c r="AQ34" s="61"/>
       <c r="AR34" s="61"/>
     </row>
-    <row r="35" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A35" s="27"/>
       <c r="B35" s="52"/>
       <c r="C35" s="46"/>
@@ -5837,7 +6005,7 @@
       <c r="AQ35" s="64"/>
       <c r="AR35" s="64"/>
     </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A36" s="38"/>
       <c r="B36" s="35"/>
       <c r="C36" s="39"/>
@@ -5931,7 +6099,7 @@
       <c r="AQ36" s="61"/>
       <c r="AR36" s="61"/>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A37" s="27"/>
       <c r="B37" s="52"/>
       <c r="C37" s="46"/>
@@ -6025,7 +6193,7 @@
       <c r="AQ37" s="64"/>
       <c r="AR37" s="64"/>
     </row>
-    <row r="38" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A38" s="38"/>
       <c r="B38" s="35"/>
       <c r="C38" s="39"/>
@@ -6119,7 +6287,7 @@
       <c r="AQ38" s="61"/>
       <c r="AR38" s="61"/>
     </row>
-    <row r="39" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A39" s="27"/>
       <c r="B39" s="52"/>
       <c r="C39" s="46"/>
@@ -6213,7 +6381,7 @@
       <c r="AQ39" s="64"/>
       <c r="AR39" s="64"/>
     </row>
-    <row r="40" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A40" s="38"/>
       <c r="B40" s="35"/>
       <c r="C40" s="39"/>
@@ -6307,7 +6475,7 @@
       <c r="AQ40" s="61"/>
       <c r="AR40" s="61"/>
     </row>
-    <row r="41" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A41" s="27"/>
       <c r="B41" s="52"/>
       <c r="C41" s="46"/>
@@ -6401,7 +6569,7 @@
       <c r="AQ41" s="64"/>
       <c r="AR41" s="64"/>
     </row>
-    <row r="42" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A42" s="38"/>
       <c r="B42" s="35"/>
       <c r="C42" s="39"/>
@@ -6495,7 +6663,7 @@
       <c r="AQ42" s="61"/>
       <c r="AR42" s="61"/>
     </row>
-    <row r="43" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A43" s="27"/>
       <c r="B43" s="52"/>
       <c r="C43" s="46"/>
@@ -6589,7 +6757,7 @@
       <c r="AQ43" s="64"/>
       <c r="AR43" s="64"/>
     </row>
-    <row r="44" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A44" s="38"/>
       <c r="B44" s="35"/>
       <c r="C44" s="39"/>
@@ -6683,7 +6851,7 @@
       <c r="AQ44" s="61"/>
       <c r="AR44" s="61"/>
     </row>
-    <row r="45" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A45" s="27"/>
       <c r="B45" s="52"/>
       <c r="C45" s="46"/>
@@ -6777,7 +6945,7 @@
       <c r="AQ45" s="64"/>
       <c r="AR45" s="64"/>
     </row>
-    <row r="46" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A46" s="38"/>
       <c r="B46" s="35"/>
       <c r="C46" s="39"/>
@@ -6871,7 +7039,7 @@
       <c r="AQ46" s="61"/>
       <c r="AR46" s="61"/>
     </row>
-    <row r="47" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A47" s="27"/>
       <c r="B47" s="52"/>
       <c r="C47" s="46"/>
@@ -6965,7 +7133,7 @@
       <c r="AQ47" s="64"/>
       <c r="AR47" s="64"/>
     </row>
-    <row r="48" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A48" s="38"/>
       <c r="B48" s="35"/>
       <c r="C48" s="39"/>
@@ -7059,7 +7227,7 @@
       <c r="AQ48" s="61"/>
       <c r="AR48" s="61"/>
     </row>
-    <row r="49" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A49" s="27"/>
       <c r="B49" s="52"/>
       <c r="C49" s="46"/>
@@ -7153,7 +7321,7 @@
       <c r="AQ49" s="64"/>
       <c r="AR49" s="64"/>
     </row>
-    <row r="50" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A50" s="38"/>
       <c r="B50" s="35"/>
       <c r="C50" s="39"/>
@@ -7247,7 +7415,7 @@
       <c r="AQ50" s="61"/>
       <c r="AR50" s="61"/>
     </row>
-    <row r="51" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A51" s="27"/>
       <c r="B51" s="52"/>
       <c r="C51" s="46"/>
@@ -7341,7 +7509,7 @@
       <c r="AQ51" s="64"/>
       <c r="AR51" s="64"/>
     </row>
-    <row r="52" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A52" s="38"/>
       <c r="B52" s="35"/>
       <c r="C52" s="39"/>
@@ -7435,7 +7603,7 @@
       <c r="AQ52" s="61"/>
       <c r="AR52" s="61"/>
     </row>
-    <row r="53" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A53" s="27"/>
       <c r="B53" s="52"/>
       <c r="C53" s="46"/>
@@ -7529,7 +7697,7 @@
       <c r="AQ53" s="64"/>
       <c r="AR53" s="64"/>
     </row>
-    <row r="54" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A54" s="38"/>
       <c r="B54" s="35"/>
       <c r="C54" s="39"/>
@@ -7623,7 +7791,7 @@
       <c r="AQ54" s="61"/>
       <c r="AR54" s="61"/>
     </row>
-    <row r="55" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A55" s="27"/>
       <c r="B55" s="52"/>
       <c r="C55" s="46"/>
@@ -7717,7 +7885,7 @@
       <c r="AQ55" s="64"/>
       <c r="AR55" s="64"/>
     </row>
-    <row r="56" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A56" s="38"/>
       <c r="B56" s="35"/>
       <c r="C56" s="39"/>
@@ -7811,7 +7979,7 @@
       <c r="AQ56" s="61"/>
       <c r="AR56" s="61"/>
     </row>
-    <row r="57" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A57" s="27"/>
       <c r="B57" s="52"/>
       <c r="C57" s="46"/>
@@ -7905,7 +8073,7 @@
       <c r="AQ57" s="64"/>
       <c r="AR57" s="64"/>
     </row>
-    <row r="58" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A58" s="38"/>
       <c r="B58" s="35"/>
       <c r="C58" s="39"/>
@@ -7999,7 +8167,7 @@
       <c r="AQ58" s="61"/>
       <c r="AR58" s="61"/>
     </row>
-    <row r="59" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A59" s="27"/>
       <c r="B59" s="52"/>
       <c r="C59" s="46"/>
@@ -8093,7 +8261,7 @@
       <c r="AQ59" s="64"/>
       <c r="AR59" s="64"/>
     </row>
-    <row r="60" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A60" s="38"/>
       <c r="B60" s="35"/>
       <c r="C60" s="39"/>
@@ -8187,7 +8355,7 @@
       <c r="AQ60" s="61"/>
       <c r="AR60" s="61"/>
     </row>
-    <row r="61" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A61" s="27"/>
       <c r="B61" s="52"/>
       <c r="C61" s="46"/>
@@ -8289,136 +8457,141 @@
   </protectedRanges>
   <phoneticPr fontId="28" type="noConversion"/>
   <conditionalFormatting sqref="AM1">
+    <cfRule type="cellIs" priority="27" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN1">
+    <cfRule type="cellIs" priority="26" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V1:AG1 V62:AG1048576">
+    <cfRule type="cellIs" priority="39" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK1:AL1 AK62:AL1048576">
+    <cfRule type="cellIs" priority="33" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL2:AL3">
+    <cfRule type="cellIs" dxfId="19" priority="31" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM2:AN3">
+    <cfRule type="cellIs" dxfId="18" priority="28" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM62:AN1048576">
+    <cfRule type="cellIs" priority="30" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ1">
+    <cfRule type="cellIs" priority="19" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH1:AI1 AH62:AI1048576">
     <cfRule type="cellIs" priority="25" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AN1">
-    <cfRule type="cellIs" priority="24" operator="notEqual">
+  <conditionalFormatting sqref="AH2:AI3">
+    <cfRule type="cellIs" dxfId="17" priority="23" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ62:AJ1048576">
+    <cfRule type="cellIs" priority="22" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V1:AG1 V62:AG1048576">
-    <cfRule type="cellIs" priority="37" operator="notEqual">
+  <conditionalFormatting sqref="V2:AG3">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ1">
+    <cfRule type="cellIs" priority="11" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK1:AL1 AK62:AL1048576">
-    <cfRule type="cellIs" priority="31" operator="notEqual">
+  <conditionalFormatting sqref="AR1">
+    <cfRule type="cellIs" priority="10" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK2:AL3">
-    <cfRule type="cellIs" dxfId="17" priority="29" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM2:AN3">
-    <cfRule type="cellIs" dxfId="16" priority="26" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM62:AN1048576">
-    <cfRule type="cellIs" priority="28" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ1">
+  <conditionalFormatting sqref="AO1:AP1 AO62:AP1048576">
     <cfRule type="cellIs" priority="17" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH1:AI1 AH62:AI1048576">
-    <cfRule type="cellIs" priority="23" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH2:AI3">
-    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ2:AJ3">
-    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ62:AJ1048576">
-    <cfRule type="cellIs" priority="20" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V2:AG3">
-    <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ1">
-    <cfRule type="cellIs" priority="9" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AR1">
-    <cfRule type="cellIs" priority="8" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO1:AP1 AO62:AP1048576">
-    <cfRule type="cellIs" priority="15" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AO2:AP3">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ2:AR3">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ62:AR1048576">
-    <cfRule type="cellIs" priority="12" operator="notEqual">
+    <cfRule type="cellIs" priority="14" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK4:AL61">
+  <conditionalFormatting sqref="AK26:AL61 AL4:AL25">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM4:AN61">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH4:AI61">
     <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AM4:AN61">
+  <conditionalFormatting sqref="AJ26:AJ61">
     <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH4:AI61">
+  <conditionalFormatting sqref="V4:AG61">
     <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ4:AJ61">
+  <conditionalFormatting sqref="AO4:AP61">
     <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V4:AG61">
+  <conditionalFormatting sqref="AQ4:AR61">
     <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AO4:AP61">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+  <conditionalFormatting sqref="AK4:AK25">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AQ4:AR61">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+  <conditionalFormatting sqref="AJ4:AJ25">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations xWindow="493" yWindow="769" count="11">
+  <dataValidations xWindow="1179" yWindow="308" count="11">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="输出信号" prompt="输出信号" sqref="Q1:T1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="指令描述符" prompt="指令助记符" sqref="B1:B1048576" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OpCode(10进制)" prompt="输入MIPS指令字的OpCode的十进制数，后续隐藏列会自动生成OpCode字段6位的二进制位" sqref="C1:C1048576" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
@@ -8443,28 +8616,28 @@
   </sheetPr>
   <dimension ref="A1:AX67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH62" sqref="AH62"/>
+      <selection pane="bottomLeft" activeCell="AJ62" sqref="AJ62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="4.88671875" style="18" hidden="1" customWidth="1"/>
-    <col min="5" max="13" width="4.6640625" style="18" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="4.21875" style="18" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="4.6640625" style="18" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="22.88671875" style="18" customWidth="1"/>
-    <col min="17" max="20" width="4.6640625" style="18" customWidth="1"/>
-    <col min="21" max="32" width="6.6640625" customWidth="1"/>
-    <col min="33" max="36" width="6.6640625" style="19" customWidth="1"/>
-    <col min="37" max="43" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.375" style="18" customWidth="1"/>
+    <col min="2" max="2" width="8.625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="9.5" style="18" customWidth="1"/>
+    <col min="4" max="4" width="4.875" style="18" hidden="1" customWidth="1"/>
+    <col min="5" max="13" width="4.625" style="18" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="4.25" style="18" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="4.625" style="18" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="22.875" style="18" customWidth="1"/>
+    <col min="17" max="20" width="4.625" style="18" customWidth="1"/>
+    <col min="21" max="32" width="6.625" customWidth="1"/>
+    <col min="33" max="36" width="6.625" style="19" customWidth="1"/>
+    <col min="37" max="43" width="6.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="17" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" s="17" customFormat="1" ht="24.75" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
@@ -8599,11 +8772,11 @@
       </c>
       <c r="AI1" s="58" t="str">
         <f>真值表!AJ1</f>
-        <v>XXX</v>
+        <v>R1_USED</v>
       </c>
       <c r="AJ1" s="58" t="str">
         <f>真值表!AK1</f>
-        <v>XXX</v>
+        <v>R2_USED</v>
       </c>
       <c r="AK1" s="58" t="str">
         <f>真值表!AL1</f>
@@ -8634,7 +8807,7 @@
         <v>XXX</v>
       </c>
     </row>
-    <row r="2" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="str">
         <f>真值表!B2</f>
         <v>SLL</v>
@@ -8773,11 +8946,11 @@
       </c>
       <c r="AI2" s="31" t="str">
         <f>IF(真值表!AJ2=1,$P2&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AJ2" s="31" t="str">
         <f>IF(真值表!AK2=1,$P2&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AK2" s="31" t="str">
         <f>IF(真值表!AL2=1,$P2&amp;"+","")</f>
@@ -8808,7 +8981,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="str">
         <f>真值表!B3</f>
         <v>SRA</v>
@@ -8947,11 +9120,11 @@
       </c>
       <c r="AI3" s="51" t="str">
         <f>IF(真值表!AJ3=1,$P3&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+</v>
       </c>
       <c r="AJ3" s="51" t="str">
         <f>IF(真值表!AK3=1,$P3&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+</v>
       </c>
       <c r="AK3" s="51" t="str">
         <f>IF(真值表!AL3=1,$P3&amp;"+","")</f>
@@ -8982,7 +9155,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="23" t="str">
         <f>真值表!B4</f>
         <v>SRL</v>
@@ -9121,11 +9294,11 @@
       </c>
       <c r="AI4" s="31" t="str">
         <f>IF(真值表!AJ4=1,$P4&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="AJ4" s="31" t="str">
         <f>IF(真值表!AK4=1,$P4&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="AK4" s="31" t="str">
         <f>IF(真值表!AL4=1,$P4&amp;"+","")</f>
@@ -9156,7 +9329,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="str">
         <f>真值表!B5</f>
         <v>ADD</v>
@@ -9295,11 +9468,11 @@
       </c>
       <c r="AI5" s="51" t="str">
         <f>IF(真值表!AJ5=1,$P5&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AJ5" s="51" t="str">
         <f>IF(真值表!AK5=1,$P5&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AK5" s="51" t="str">
         <f>IF(真值表!AL5=1,$P5&amp;"+","")</f>
@@ -9330,7 +9503,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="str">
         <f>真值表!B6</f>
         <v>ADDU</v>
@@ -9469,11 +9642,11 @@
       </c>
       <c r="AI6" s="31" t="str">
         <f>IF(真值表!AJ6=1,$P6&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+</v>
       </c>
       <c r="AJ6" s="31" t="str">
         <f>IF(真值表!AK6=1,$P6&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+</v>
       </c>
       <c r="AK6" s="31" t="str">
         <f>IF(真值表!AL6=1,$P6&amp;"+","")</f>
@@ -9504,7 +9677,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="str">
         <f>真值表!B7</f>
         <v>SUB</v>
@@ -9643,11 +9816,11 @@
       </c>
       <c r="AI7" s="51" t="str">
         <f>IF(真值表!AJ7=1,$P7&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="AJ7" s="51" t="str">
         <f>IF(真值表!AK7=1,$P7&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="AK7" s="51" t="str">
         <f>IF(真值表!AL7=1,$P7&amp;"+","")</f>
@@ -9678,7 +9851,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="str">
         <f>真值表!B8</f>
         <v>AND</v>
@@ -9817,11 +9990,11 @@
       </c>
       <c r="AI8" s="31" t="str">
         <f>IF(真值表!AJ8=1,$P8&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AJ8" s="31" t="str">
         <f>IF(真值表!AK8=1,$P8&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AK8" s="31" t="str">
         <f>IF(真值表!AL8=1,$P8&amp;"+","")</f>
@@ -9852,7 +10025,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="str">
         <f>真值表!B9</f>
         <v>OR</v>
@@ -9991,11 +10164,11 @@
       </c>
       <c r="AI9" s="51" t="str">
         <f>IF(真值表!AJ9=1,$P9&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp; F0+</v>
       </c>
       <c r="AJ9" s="51" t="str">
         <f>IF(真值表!AK9=1,$P9&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp; F0+</v>
       </c>
       <c r="AK9" s="51" t="str">
         <f>IF(真值表!AL9=1,$P9&amp;"+","")</f>
@@ -10026,7 +10199,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="str">
         <f>真值表!B10</f>
         <v>NOR</v>
@@ -10165,11 +10338,11 @@
       </c>
       <c r="AI10" s="31" t="str">
         <f>IF(真值表!AJ10=1,$P10&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+</v>
       </c>
       <c r="AJ10" s="31" t="str">
         <f>IF(真值表!AK10=1,$P10&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+</v>
       </c>
       <c r="AK10" s="31" t="str">
         <f>IF(真值表!AL10=1,$P10&amp;"+","")</f>
@@ -10200,7 +10373,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="str">
         <f>真值表!B11</f>
         <v>SLT</v>
@@ -10339,11 +10512,11 @@
       </c>
       <c r="AI11" s="51" t="str">
         <f>IF(真值表!AJ11=1,$P11&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="AJ11" s="51" t="str">
         <f>IF(真值表!AK11=1,$P11&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="AK11" s="51" t="str">
         <f>IF(真值表!AL11=1,$P11&amp;"+","")</f>
@@ -10374,7 +10547,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="str">
         <f>真值表!B12</f>
         <v>SLTU</v>
@@ -10513,11 +10686,11 @@
       </c>
       <c r="AI12" s="31" t="str">
         <f>IF(真值表!AJ12=1,$P12&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+</v>
       </c>
       <c r="AJ12" s="31" t="str">
         <f>IF(真值表!AK12=1,$P12&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+</v>
       </c>
       <c r="AK12" s="31" t="str">
         <f>IF(真值表!AL12=1,$P12&amp;"+","")</f>
@@ -10548,7 +10721,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="str">
         <f>真值表!B13</f>
         <v>JR</v>
@@ -10687,7 +10860,7 @@
       </c>
       <c r="AI13" s="51" t="str">
         <f>IF(真值表!AJ13=1,$P13&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp;~F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AJ13" s="51" t="str">
         <f>IF(真值表!AK13=1,$P13&amp;"+","")</f>
@@ -10722,7 +10895,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="23" t="str">
         <f>真值表!B14</f>
         <v>SYSCALL</v>
@@ -10861,11 +11034,11 @@
       </c>
       <c r="AI14" s="31" t="str">
         <f>IF(真值表!AJ14=1,$P14&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp; F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AJ14" s="31" t="str">
         <f>IF(真值表!AK14=1,$P14&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp; F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AK14" s="31" t="str">
         <f>IF(真值表!AL14=1,$P14&amp;"+","")</f>
@@ -10896,7 +11069,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="str">
         <f>真值表!B15</f>
         <v>J</v>
@@ -11070,7 +11243,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="23" t="str">
         <f>真值表!B16</f>
         <v>JAL</v>
@@ -11244,7 +11417,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="str">
         <f>真值表!B17</f>
         <v>BEQ</v>
@@ -11383,11 +11556,11 @@
       </c>
       <c r="AI17" s="51" t="str">
         <f>IF(真值表!AJ17=1,$P17&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="AJ17" s="51" t="str">
         <f>IF(真值表!AK17=1,$P17&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="AK17" s="51" t="str">
         <f>IF(真值表!AL17=1,$P17&amp;"+","")</f>
@@ -11418,7 +11591,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="23" t="str">
         <f>真值表!B18</f>
         <v>BNE</v>
@@ -11557,11 +11730,11 @@
       </c>
       <c r="AI18" s="31" t="str">
         <f>IF(真值表!AJ18=1,$P18&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="AJ18" s="31" t="str">
         <f>IF(真值表!AK18=1,$P18&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="AK18" s="31" t="str">
         <f>IF(真值表!AL18=1,$P18&amp;"+","")</f>
@@ -11592,7 +11765,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="str">
         <f>真值表!B19</f>
         <v>ADDI</v>
@@ -11731,7 +11904,7 @@
       </c>
       <c r="AI19" s="51" t="str">
         <f>IF(真值表!AJ19=1,$P19&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="AJ19" s="51" t="str">
         <f>IF(真值表!AK19=1,$P19&amp;"+","")</f>
@@ -11766,7 +11939,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A20" s="23" t="str">
         <f>真值表!B20</f>
         <v>ANDI</v>
@@ -11905,7 +12078,7 @@
       </c>
       <c r="AI20" s="31" t="str">
         <f>IF(真值表!AJ20=1,$P20&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="AJ20" s="31" t="str">
         <f>IF(真值表!AK20=1,$P20&amp;"+","")</f>
@@ -11940,7 +12113,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="str">
         <f>真值表!B21</f>
         <v>ADDIU</v>
@@ -12079,7 +12252,7 @@
       </c>
       <c r="AI21" s="51" t="str">
         <f>IF(真值表!AJ21=1,$P21&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="AJ21" s="51" t="str">
         <f>IF(真值表!AK21=1,$P21&amp;"+","")</f>
@@ -12114,7 +12287,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="23" t="str">
         <f>真值表!B22</f>
         <v>SLTI</v>
@@ -12253,7 +12426,7 @@
       </c>
       <c r="AI22" s="31" t="str">
         <f>IF(真值表!AJ22=1,$P22&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+</v>
       </c>
       <c r="AJ22" s="31" t="str">
         <f>IF(真值表!AK22=1,$P22&amp;"+","")</f>
@@ -12288,7 +12461,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="str">
         <f>真值表!B23</f>
         <v>ORI</v>
@@ -12427,7 +12600,7 @@
       </c>
       <c r="AI23" s="51" t="str">
         <f>IF(真值表!AJ23=1,$P23&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="AJ23" s="51" t="str">
         <f>IF(真值表!AK23=1,$P23&amp;"+","")</f>
@@ -12462,7 +12635,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="23" t="str">
         <f>真值表!B24</f>
         <v>LW</v>
@@ -12601,11 +12774,11 @@
       </c>
       <c r="AI24" s="31" t="str">
         <f>IF(真值表!AJ24=1,$P24&amp;"+","")</f>
-        <v/>
+        <v xml:space="preserve"> OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="AJ24" s="31" t="str">
         <f>IF(真值表!AK24=1,$P24&amp;"+","")</f>
-        <v/>
+        <v xml:space="preserve"> OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="AK24" s="31" t="str">
         <f>IF(真值表!AL24=1,$P24&amp;"+","")</f>
@@ -12636,7 +12809,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A25" s="27" t="str">
         <f>真值表!B25</f>
         <v>SW</v>
@@ -12775,11 +12948,11 @@
       </c>
       <c r="AI25" s="51" t="str">
         <f>IF(真值表!AJ25=1,$P25&amp;"+","")</f>
-        <v/>
+        <v xml:space="preserve"> OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="AJ25" s="51" t="str">
         <f>IF(真值表!AK25=1,$P25&amp;"+","")</f>
-        <v/>
+        <v xml:space="preserve"> OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="AK25" s="51" t="str">
         <f>IF(真值表!AL25=1,$P25&amp;"+","")</f>
@@ -12810,7 +12983,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A26" s="23" t="str">
         <f>真值表!B26</f>
         <v>XOR</v>
@@ -12949,11 +13122,11 @@
       </c>
       <c r="AI26" s="31" t="str">
         <f>IF(真值表!AJ26=1,$P26&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="AJ26" s="31" t="str">
         <f>IF(真值表!AK26=1,$P26&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="AK26" s="31" t="str">
         <f>IF(真值表!AL26=1,$P26&amp;"+","")</f>
@@ -12984,7 +13157,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A27" s="27" t="str">
         <f>真值表!B27</f>
         <v>XORI</v>
@@ -13123,7 +13296,7 @@
       </c>
       <c r="AI27" s="51" t="str">
         <f>IF(真值表!AJ27=1,$P27&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp; OP2&amp; OP1&amp;~OP0+</v>
       </c>
       <c r="AJ27" s="51" t="str">
         <f>IF(真值表!AK27=1,$P27&amp;"+","")</f>
@@ -13158,7 +13331,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A28" s="23" t="str">
         <f>真值表!B28</f>
         <v>LHU</v>
@@ -13297,11 +13470,11 @@
       </c>
       <c r="AI28" s="31" t="str">
         <f>IF(真值表!AJ28=1,$P28&amp;"+","")</f>
-        <v/>
+        <v xml:space="preserve"> OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="AJ28" s="31" t="str">
         <f>IF(真值表!AK28=1,$P28&amp;"+","")</f>
-        <v/>
+        <v xml:space="preserve"> OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="AK28" s="31" t="str">
         <f>IF(真值表!AL28=1,$P28&amp;"+","")</f>
@@ -13332,7 +13505,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A29" s="27" t="str">
         <f>真值表!B29</f>
         <v>BGTZ</v>
@@ -13471,7 +13644,7 @@
       </c>
       <c r="AI29" s="51" t="str">
         <f>IF(真值表!AJ29=1,$P29&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="AJ29" s="51" t="str">
         <f>IF(真值表!AK29=1,$P29&amp;"+","")</f>
@@ -13506,7 +13679,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A30" s="23">
         <f>真值表!B30</f>
         <v>0</v>
@@ -13680,7 +13853,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A31" s="27">
         <f>真值表!B31</f>
         <v>0</v>
@@ -13854,7 +14027,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:43" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:43" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A32" s="23">
         <f>真值表!B32</f>
         <v>0</v>
@@ -14028,7 +14201,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:43" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:43" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="27">
         <f>真值表!B33</f>
         <v>0</v>
@@ -14202,7 +14375,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:43" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:43" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="23">
         <f>真值表!B34</f>
         <v>0</v>
@@ -14376,7 +14549,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:43" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:43" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="27">
         <f>真值表!B35</f>
         <v>0</v>
@@ -14550,7 +14723,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:43" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:43" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="23">
         <f>真值表!B36</f>
         <v>0</v>
@@ -14724,7 +14897,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:43" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:43" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="27">
         <f>真值表!B37</f>
         <v>0</v>
@@ -14898,7 +15071,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:43" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:43" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="23">
         <f>真值表!B38</f>
         <v>0</v>
@@ -15072,7 +15245,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:43" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:43" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="27">
         <f>真值表!B39</f>
         <v>0</v>
@@ -15246,7 +15419,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:43" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:43" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="23">
         <f>真值表!B40</f>
         <v>0</v>
@@ -15420,7 +15593,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:43" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:43" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="27">
         <f>真值表!B41</f>
         <v>0</v>
@@ -15594,7 +15767,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:43" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:43" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="23">
         <f>真值表!B42</f>
         <v>0</v>
@@ -15768,7 +15941,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:43" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:43" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="27">
         <f>真值表!B43</f>
         <v>0</v>
@@ -15942,7 +16115,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:43" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:43" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="23">
         <f>真值表!B44</f>
         <v>0</v>
@@ -16116,7 +16289,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:43" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:43" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="27">
         <f>真值表!B45</f>
         <v>0</v>
@@ -16290,7 +16463,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:43" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:43" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="23">
         <f>真值表!B46</f>
         <v>0</v>
@@ -16464,7 +16637,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:43" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:43" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="27">
         <f>真值表!B47</f>
         <v>0</v>
@@ -16638,7 +16811,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:43" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:43" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="23">
         <f>真值表!B48</f>
         <v>0</v>
@@ -16812,7 +16985,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:50" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:50" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="27">
         <f>真值表!B49</f>
         <v>0</v>
@@ -16986,7 +17159,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:50" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:50" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="23">
         <f>真值表!B50</f>
         <v>0</v>
@@ -17160,7 +17333,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:50" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:50" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="27">
         <f>真值表!B51</f>
         <v>0</v>
@@ -17334,7 +17507,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:50" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:50" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="23">
         <f>真值表!B52</f>
         <v>0</v>
@@ -17508,7 +17681,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:50" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:50" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="27">
         <f>真值表!B53</f>
         <v>0</v>
@@ -17682,7 +17855,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:50" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:50" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="23">
         <f>真值表!B54</f>
         <v>0</v>
@@ -17856,7 +18029,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:50" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:50" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="27">
         <f>真值表!B55</f>
         <v>0</v>
@@ -18030,7 +18203,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:50" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:50" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="23">
         <f>真值表!B56</f>
         <v>0</v>
@@ -18204,7 +18377,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:50" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:50" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="27">
         <f>真值表!B57</f>
         <v>0</v>
@@ -18378,7 +18551,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:50" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:50" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="23">
         <f>真值表!B58</f>
         <v>0</v>
@@ -18552,7 +18725,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:50" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:50" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="27">
         <f>真值表!B59</f>
         <v>0</v>
@@ -18726,7 +18899,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:50" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:50" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="23">
         <f>真值表!B60</f>
         <v>0</v>
@@ -18900,7 +19073,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:50" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:50" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="27">
         <f>真值表!B61</f>
         <v>0</v>
@@ -19074,7 +19247,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:50" ht="16.2" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:50" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="68" t="s">
         <v>113</v>
       </c>
@@ -19167,11 +19340,11 @@
       </c>
       <c r="AI62" s="36" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp; OP0+ OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp; OP1&amp;~OP0+ OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp; OP1&amp; OP0</v>
       </c>
       <c r="AJ62" s="36" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+ OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp;~F0+ OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0</v>
       </c>
       <c r="AK62" s="36" t="str">
         <f t="shared" si="1"/>
@@ -19202,7 +19375,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:50" hidden="1" x14ac:dyDescent="0.2">
       <c r="Q63" t="str">
         <f t="shared" ref="Q63:AQ63" si="2">CONCATENATE(Q2,Q3,Q4,Q5,Q6,Q7,Q8,Q9,Q10,Q11,Q12,Q13,Q14,Q15,Q16,Q17,Q18,Q19,Q20,Q21,Q22,Q23,Q24,Q25,Q26,Q27,Q28,Q29,Q30,Q31,Q32,Q33,Q34,Q35,Q36,Q37,Q38,Q39,Q40,Q41,Q42,Q43,Q44,Q45,Q46,Q47,Q48,Q49,Q50,Q51,Q52,Q53,Q54,Q55,Q56,Q57,
 )</f>
@@ -19278,11 +19451,11 @@
       </c>
       <c r="AI63" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp; OP0+ OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp; OP1&amp;~OP0+ OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="AJ63" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+ OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp;~F0+ OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="AK63" t="str">
         <f t="shared" si="2"/>
@@ -19342,7 +19515,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="18:32" ht="20.399999999999999" x14ac:dyDescent="0.45">
+    <row r="65" spans="18:32" ht="21" x14ac:dyDescent="0.4">
       <c r="V65" s="69" t="s">
         <v>115</v>
       </c>
@@ -19357,7 +19530,7 @@
       <c r="AE65" s="69"/>
       <c r="AF65" s="69"/>
     </row>
-    <row r="67" spans="18:32" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="18:32" ht="15" x14ac:dyDescent="0.2">
       <c r="R67" s="37" t="s">
         <v>114</v>
       </c>
@@ -19370,22 +19543,22 @@
   </mergeCells>
   <phoneticPr fontId="28" type="noConversion"/>
   <conditionalFormatting sqref="P1 Q63:AX63 Q62:AQ62">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q64:AF64 Q1:AF1 Q68:AF1048576 Q67 S67:AF67 Q66:AF66 Q65:V65 Q2:AQ3">
-    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG64:AJ1048576 AG1:AQ1">
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4:AQ61">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19420,14 +19593,14 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.21875" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="49.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.25" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="49.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
@@ -19471,7 +19644,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>63</v>
       </c>
@@ -19598,14 +19771,14 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="56.109375" customWidth="1"/>
+    <col min="4" max="4" width="56.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -19619,7 +19792,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -19633,7 +19806,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -19647,7 +19820,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -19661,7 +19834,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -19675,7 +19848,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -19689,7 +19862,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -19703,7 +19876,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -19717,7 +19890,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -19731,7 +19904,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -19745,7 +19918,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -19759,7 +19932,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -19773,7 +19946,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -19787,7 +19960,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>

</xml_diff>